<commit_message>
atualização de dependencias do projeto com erro no .net
</commit_message>
<xml_diff>
--- a/Processamento Inteligente de Documentos/Documentos/Extracao/Fatura2.pdf.xlsx
+++ b/Processamento Inteligente de Documentos/Documentos/Extracao/Fatura2.pdf.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <x:si>
     <x:t>Empresa</x:t>
   </x:si>
@@ -60,7 +60,10 @@
     <x:t>Montante</x:t>
   </x:si>
   <x:si>
-    <x:t>Starter Shared Hosting - (28/09/2016 - 27/10/2016) Hosting Location: United Kingdom (UK)</x:t>
+    <x:t>Starter Shared Hosting - (28/09/2016 - 27/10/2016)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hosting Location: United Kingdom (UK)</x:t>
   </x:si>
   <x:si>
     <x:t>Late Fee (Added 02/10/2016)</x:t>
@@ -555,8 +558,13 @@
       <x:c r="A3" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
         <x:v>15</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -599,8 +607,13 @@
       <x:c r="A3" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
         <x:v>15</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>